<commit_message>
Fixing bugs in statistics
</commit_message>
<xml_diff>
--- a/comp.xlsx
+++ b/comp.xlsx
@@ -13574,7 +13574,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Девки
 не
@@ -13591,7 +13590,6 @@
         <sz val="10"/>
         <rFont val="AR PL UMing CN"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ツ</t>
     </r>
@@ -13602,7 +13600,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Девки
 не
@@ -13618,7 +13615,6 @@
         <sz val="10"/>
         <rFont val="AR PL UMing CN"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ツ</t>
     </r>
@@ -21341,16 +21337,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -21371,7 +21367,6 @@
       <sz val="10"/>
       <name val="AR PL UMing CN"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -21416,7 +21411,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -21437,6 +21432,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -21454,12 +21453,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T883"/>
+  <dimension ref="A1:T889"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A882" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K894" activeCellId="0" sqref="K894"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A498" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C499" activeCellId="0" sqref="C499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25483,7 +25482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="n">
         <v>190</v>
       </c>
@@ -37241,7 +37240,7 @@
       <c r="J753" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L753" s="1" t="n">
+      <c r="K753" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T753" s="1" t="s">
@@ -38182,7 +38181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="798" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="798" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A798" s="1" t="n">
         <v>796</v>
       </c>
@@ -39963,11 +39962,11 @@
       </c>
       <c r="K883" s="1" t="n">
         <f aca="false">SUM(K1:K882)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L883" s="1" t="n">
         <f aca="false">SUM(L1:L882)</f>
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M883" s="1" t="n">
         <f aca="false">SUM(M1:M882)</f>
@@ -39988,6 +39987,59 @@
       <c r="Q883" s="1" t="n">
         <f aca="false">SUM(Q1:Q882)</f>
         <v>56</v>
+      </c>
+    </row>
+    <row r="884" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F884" s="5" t="n">
+        <f aca="false">F883/881</f>
+        <v>0.692395005675369</v>
+      </c>
+      <c r="G884" s="5" t="n">
+        <f aca="false">G883/881</f>
+        <v>0.0192962542565267</v>
+      </c>
+      <c r="H884" s="5" t="n">
+        <f aca="false">H883/881</f>
+        <v>0.00227014755959137</v>
+      </c>
+      <c r="I884" s="5" t="n">
+        <f aca="false">I883/881</f>
+        <v>0.0113507377979569</v>
+      </c>
+      <c r="J884" s="5"/>
+      <c r="K884" s="5" t="n">
+        <f aca="false">K883/881</f>
+        <v>0.0317820658342792</v>
+      </c>
+      <c r="L884" s="5" t="n">
+        <f aca="false">L883/881</f>
+        <v>0.172531214528944</v>
+      </c>
+      <c r="M884" s="5" t="n">
+        <f aca="false">M883/881</f>
+        <v>0.0113507377979569</v>
+      </c>
+      <c r="N884" s="5" t="n">
+        <f aca="false">N883/881</f>
+        <v>0.0147559591373439</v>
+      </c>
+      <c r="O884" s="5" t="n">
+        <f aca="false">O883/881</f>
+        <v>0.0147559591373439</v>
+      </c>
+      <c r="P884" s="5" t="n">
+        <f aca="false">P883/881</f>
+        <v>0.00113507377979569</v>
+      </c>
+      <c r="Q884" s="5" t="n">
+        <f aca="false">Q883/881</f>
+        <v>0.0635641316685585</v>
+      </c>
+    </row>
+    <row r="889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H889" s="1" t="n">
+        <f aca="false">SUM(F883:I883)+SUM(K883:O883)+Q883</f>
+        <v>911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating xlsx file for sentences with errors (and fixing some bugs in comp.xlsx)
</commit_message>
<xml_diff>
--- a/comp.xlsx
+++ b/comp.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2662" uniqueCount="1784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2663" uniqueCount="1785">
   <si>
     <t xml:space="preserve">gold_text</t>
   </si>
@@ -13574,6 +13574,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Девки
 не
@@ -13590,6 +13591,7 @@
         <sz val="10"/>
         <rFont val="AR PL UMing CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ツ</t>
     </r>
@@ -13600,6 +13602,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Девки
 не
@@ -13615,6 +13618,7 @@
         <sz val="10"/>
         <rFont val="AR PL UMing CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ツ</t>
     </r>
@@ -16845,6 +16849,9 @@
   </si>
   <si>
     <t xml:space="preserve">(19, 16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!!!!! → !!!</t>
   </si>
   <si>
     <t xml:space="preserve">ЭВЕЛИНА
@@ -21347,6 +21354,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -21367,6 +21375,7 @@
       <sz val="10"/>
       <name val="AR PL UMing CN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -21455,10 +21464,10 @@
   </sheetPr>
   <dimension ref="A1:T889"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A498" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C499" activeCellId="0" sqref="C499"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A882" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="R882" activeCellId="0" sqref="R882"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22270,7 +22279,7 @@
       <c r="N36" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="P36" s="1" t="n">
+      <c r="O36" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -36940,19 +36949,25 @@
       <c r="L738" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="O738" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T738" s="1" t="s">
+        <v>1498</v>
+      </c>
     </row>
     <row r="739" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A739" s="1" t="n">
         <v>737</v>
       </c>
       <c r="B739" s="3" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
       <c r="C739" s="3" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="D739" s="1" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="E739" s="1" t="n">
         <v>1</v>
@@ -36972,10 +36987,10 @@
         <v>738</v>
       </c>
       <c r="B740" s="3" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="C740" s="3" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="D740" s="1" t="s">
         <v>241</v>
@@ -36989,10 +37004,10 @@
         <v>739</v>
       </c>
       <c r="B741" s="3" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="C741" s="3" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="D741" s="1" t="s">
         <v>34</v>
@@ -37009,10 +37024,10 @@
         <v>740</v>
       </c>
       <c r="B742" s="3" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="C742" s="3" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="D742" s="1" t="s">
         <v>69</v>
@@ -37029,10 +37044,10 @@
         <v>741</v>
       </c>
       <c r="B743" s="3" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="C743" s="3" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="D743" s="1" t="s">
         <v>489</v>
@@ -37052,10 +37067,10 @@
         <v>742</v>
       </c>
       <c r="B744" s="3" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="C744" s="3" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
       <c r="D744" s="1" t="s">
         <v>401</v>
@@ -37072,10 +37087,10 @@
         <v>743</v>
       </c>
       <c r="B745" s="3" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="C745" s="3" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
       <c r="D745" s="1" t="s">
         <v>489</v>
@@ -37089,10 +37104,10 @@
         <v>744</v>
       </c>
       <c r="B746" s="3" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="C746" s="3" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="D746" s="1" t="s">
         <v>367</v>
@@ -37106,10 +37121,10 @@
         <v>745</v>
       </c>
       <c r="B747" s="3" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="C747" s="3" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
       <c r="D747" s="1" t="s">
         <v>40</v>
@@ -37126,10 +37141,10 @@
         <v>746</v>
       </c>
       <c r="B748" s="3" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
       <c r="C748" s="3" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="D748" s="1" t="s">
         <v>37</v>
@@ -37146,10 +37161,10 @@
         <v>747</v>
       </c>
       <c r="B749" s="3" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="C749" s="3" t="s">
-        <v>1516</v>
+        <v>1517</v>
       </c>
       <c r="D749" s="1" t="s">
         <v>526</v>
@@ -37163,10 +37178,10 @@
         <v>748</v>
       </c>
       <c r="B750" s="3" t="s">
-        <v>1517</v>
+        <v>1518</v>
       </c>
       <c r="C750" s="3" t="s">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="D750" s="1" t="s">
         <v>34</v>
@@ -37183,10 +37198,10 @@
         <v>749</v>
       </c>
       <c r="B751" s="3" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="C751" s="3" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
       <c r="D751" s="1" t="s">
         <v>64</v>
@@ -37203,10 +37218,10 @@
         <v>750</v>
       </c>
       <c r="B752" s="3" t="s">
-        <v>1521</v>
+        <v>1522</v>
       </c>
       <c r="C752" s="3" t="s">
-        <v>1522</v>
+        <v>1523</v>
       </c>
       <c r="D752" s="1" t="s">
         <v>37</v>
@@ -37223,10 +37238,10 @@
         <v>751</v>
       </c>
       <c r="B753" s="3" t="s">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="C753" s="3" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="D753" s="1" t="s">
         <v>34</v>
@@ -37244,7 +37259,7 @@
         <v>1</v>
       </c>
       <c r="T753" s="1" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="754" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37252,10 +37267,10 @@
         <v>752</v>
       </c>
       <c r="B754" s="3" t="s">
-        <v>1526</v>
+        <v>1527</v>
       </c>
       <c r="C754" s="3" t="s">
-        <v>1527</v>
+        <v>1528</v>
       </c>
       <c r="D754" s="1" t="s">
         <v>24</v>
@@ -37272,10 +37287,10 @@
         <v>753</v>
       </c>
       <c r="B755" s="3" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="C755" s="3" t="s">
-        <v>1529</v>
+        <v>1530</v>
       </c>
       <c r="D755" s="1" t="s">
         <v>64</v>
@@ -37292,10 +37307,10 @@
         <v>754</v>
       </c>
       <c r="B756" s="3" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="C756" s="3" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="D756" s="1" t="s">
         <v>18</v>
@@ -37312,7 +37327,7 @@
         <v>755</v>
       </c>
       <c r="B757" s="3" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="C757" s="1" t="s">
         <v>403</v>
@@ -37332,10 +37347,10 @@
         <v>756</v>
       </c>
       <c r="B758" s="3" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="C758" s="3" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="D758" s="1" t="s">
         <v>64</v>
@@ -37352,10 +37367,10 @@
         <v>757</v>
       </c>
       <c r="B759" s="3" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="C759" s="3" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D759" s="1" t="s">
         <v>112</v>
@@ -37369,10 +37384,10 @@
         <v>758</v>
       </c>
       <c r="B760" s="3" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="C760" s="3" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="D760" s="1" t="s">
         <v>489</v>
@@ -37386,10 +37401,10 @@
         <v>759</v>
       </c>
       <c r="B761" s="3" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="C761" s="3" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="D761" s="1" t="s">
         <v>110</v>
@@ -37406,10 +37421,10 @@
         <v>760</v>
       </c>
       <c r="B762" s="3" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="C762" s="3" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="D762" s="1" t="s">
         <v>37</v>
@@ -37426,10 +37441,10 @@
         <v>761</v>
       </c>
       <c r="B763" s="3" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="C763" s="3" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="D763" s="1" t="s">
         <v>98</v>
@@ -37446,13 +37461,13 @@
         <v>762</v>
       </c>
       <c r="B764" s="3" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="C764" s="3" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="D764" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="E764" s="1" t="n">
         <v>1</v>
@@ -37463,10 +37478,10 @@
         <v>763</v>
       </c>
       <c r="B765" s="3" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="C765" s="3" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D765" s="1" t="s">
         <v>141</v>
@@ -37483,10 +37498,10 @@
         <v>764</v>
       </c>
       <c r="B766" s="3" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="C766" s="3" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="D766" s="1" t="s">
         <v>69</v>
@@ -37503,10 +37518,10 @@
         <v>765</v>
       </c>
       <c r="B767" s="3" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="C767" s="3" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="D767" s="1" t="s">
         <v>61</v>
@@ -37523,13 +37538,13 @@
         <v>766</v>
       </c>
       <c r="B768" s="3" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="C768" s="3" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D768" s="1" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="E768" s="1" t="n">
         <v>1</v>
@@ -37549,10 +37564,10 @@
         <v>767</v>
       </c>
       <c r="B769" s="3" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="C769" s="3" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="D769" s="1" t="s">
         <v>115</v>
@@ -37569,10 +37584,10 @@
         <v>768</v>
       </c>
       <c r="B770" s="3" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="C770" s="3" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D770" s="1" t="s">
         <v>24</v>
@@ -37589,10 +37604,10 @@
         <v>769</v>
       </c>
       <c r="B771" s="3" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="C771" s="3" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D771" s="1" t="s">
         <v>34</v>
@@ -37609,10 +37624,10 @@
         <v>770</v>
       </c>
       <c r="B772" s="3" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="C772" s="3" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="D772" s="1" t="s">
         <v>1483</v>
@@ -37635,10 +37650,10 @@
         <v>771</v>
       </c>
       <c r="B773" s="3" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="C773" s="3" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D773" s="1" t="s">
         <v>52</v>
@@ -37661,10 +37676,10 @@
         <v>772</v>
       </c>
       <c r="B774" s="3" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="C774" s="3" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="D774" s="1" t="s">
         <v>105</v>
@@ -37681,10 +37696,10 @@
         <v>773</v>
       </c>
       <c r="B775" s="3" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="C775" s="3" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="D775" s="1" t="s">
         <v>34</v>
@@ -37707,10 +37722,10 @@
         <v>774</v>
       </c>
       <c r="B776" s="3" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="C776" s="3" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="D776" s="1" t="s">
         <v>115</v>
@@ -37727,10 +37742,10 @@
         <v>775</v>
       </c>
       <c r="B777" s="3" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="C777" s="3" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="D777" s="1" t="s">
         <v>37</v>
@@ -37747,10 +37762,10 @@
         <v>776</v>
       </c>
       <c r="B778" s="3" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="C778" s="3" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D778" s="1" t="s">
         <v>1483</v>
@@ -37773,10 +37788,10 @@
         <v>777</v>
       </c>
       <c r="B779" s="3" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="C779" s="3" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="D779" s="1" t="s">
         <v>241</v>
@@ -37790,10 +37805,10 @@
         <v>778</v>
       </c>
       <c r="B780" s="3" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="C780" s="3" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="D780" s="1" t="s">
         <v>297</v>
@@ -37816,10 +37831,10 @@
         <v>779</v>
       </c>
       <c r="B781" s="3" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="C781" s="3" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="D781" s="1" t="s">
         <v>110</v>
@@ -37836,13 +37851,13 @@
         <v>780</v>
       </c>
       <c r="B782" s="3" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="C782" s="3" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="D782" s="1" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="E782" s="1" t="n">
         <v>1</v>
@@ -37853,10 +37868,10 @@
         <v>781</v>
       </c>
       <c r="B783" s="3" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="C783" s="3" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="D783" s="1" t="s">
         <v>137</v>
@@ -37874,7 +37889,7 @@
         <v>1</v>
       </c>
       <c r="T783" s="1" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="784" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37882,10 +37897,10 @@
         <v>782</v>
       </c>
       <c r="B784" s="3" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="C784" s="1" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="D784" s="1" t="s">
         <v>44</v>
@@ -37902,10 +37917,10 @@
         <v>783</v>
       </c>
       <c r="B785" s="3" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="C785" s="3" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="D785" s="1" t="s">
         <v>24</v>
@@ -37922,10 +37937,10 @@
         <v>784</v>
       </c>
       <c r="B786" s="3" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="C786" s="3" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="D786" s="1" t="s">
         <v>265</v>
@@ -37939,10 +37954,10 @@
         <v>785</v>
       </c>
       <c r="B787" s="3" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="C787" s="3" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="D787" s="1" t="s">
         <v>37</v>
@@ -37959,10 +37974,10 @@
         <v>786</v>
       </c>
       <c r="B788" s="3" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="C788" s="3" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="D788" s="1" t="s">
         <v>52</v>
@@ -37985,10 +38000,10 @@
         <v>787</v>
       </c>
       <c r="B789" s="3" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="C789" s="3" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D789" s="1" t="s">
         <v>98</v>
@@ -38005,10 +38020,10 @@
         <v>788</v>
       </c>
       <c r="B790" s="3" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="C790" s="3" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="D790" s="1" t="s">
         <v>131</v>
@@ -38028,13 +38043,13 @@
         <v>789</v>
       </c>
       <c r="B791" s="3" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="C791" s="1" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="D791" s="1" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="E791" s="1" t="n">
         <v>1</v>
@@ -38048,13 +38063,13 @@
         <v>790</v>
       </c>
       <c r="B792" s="3" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="C792" s="3" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="D792" s="1" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="E792" s="1" t="n">
         <v>1</v>
@@ -38074,10 +38089,10 @@
         <v>791</v>
       </c>
       <c r="B793" s="3" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="C793" s="3" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="D793" s="1" t="s">
         <v>69</v>
@@ -38094,13 +38109,13 @@
         <v>792</v>
       </c>
       <c r="B794" s="3" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="C794" s="3" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="D794" s="1" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="E794" s="1" t="n">
         <v>1</v>
@@ -38112,7 +38127,7 @@
         <v>1</v>
       </c>
       <c r="T794" s="1" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="795" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38120,10 +38135,10 @@
         <v>793</v>
       </c>
       <c r="B795" s="3" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="C795" s="3" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="D795" s="1" t="s">
         <v>563</v>
@@ -38140,10 +38155,10 @@
         <v>794</v>
       </c>
       <c r="B796" s="3" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="C796" s="3" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="D796" s="1" t="s">
         <v>37</v>
@@ -38160,10 +38175,10 @@
         <v>795</v>
       </c>
       <c r="B797" s="3" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="C797" s="3" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="D797" s="1" t="s">
         <v>64</v>
@@ -38186,10 +38201,10 @@
         <v>796</v>
       </c>
       <c r="B798" s="3" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="C798" s="3" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="D798" s="1" t="s">
         <v>69</v>
@@ -38206,10 +38221,10 @@
         <v>797</v>
       </c>
       <c r="B799" s="3" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="C799" s="3" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="D799" s="1" t="s">
         <v>40</v>
@@ -38226,7 +38241,7 @@
         <v>798</v>
       </c>
       <c r="B800" s="3" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="C800" s="1" t="s">
         <v>522</v>
@@ -38246,10 +38261,10 @@
         <v>799</v>
       </c>
       <c r="B801" s="3" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="C801" s="3" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="D801" s="1" t="s">
         <v>115</v>
@@ -38266,10 +38281,10 @@
         <v>800</v>
       </c>
       <c r="B802" s="3" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="C802" s="3" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="D802" s="1" t="s">
         <v>69</v>
@@ -38286,10 +38301,10 @@
         <v>801</v>
       </c>
       <c r="B803" s="3" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="C803" s="3" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="D803" s="1" t="s">
         <v>37</v>
@@ -38306,10 +38321,10 @@
         <v>802</v>
       </c>
       <c r="B804" s="3" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="C804" s="3" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="D804" s="1" t="s">
         <v>367</v>
@@ -38335,10 +38350,10 @@
         <v>803</v>
       </c>
       <c r="B805" s="3" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="C805" s="3" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="D805" s="1" t="s">
         <v>37</v>
@@ -38355,10 +38370,10 @@
         <v>804</v>
       </c>
       <c r="B806" s="3" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="C806" s="3" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="D806" s="1" t="s">
         <v>141</v>
@@ -38375,13 +38390,13 @@
         <v>805</v>
       </c>
       <c r="B807" s="3" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="C807" s="3" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="D807" s="1" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="E807" s="1" t="n">
         <v>1</v>
@@ -38398,10 +38413,10 @@
         <v>806</v>
       </c>
       <c r="B808" s="3" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="C808" s="3" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="D808" s="1" t="s">
         <v>504</v>
@@ -38424,10 +38439,10 @@
         <v>807</v>
       </c>
       <c r="B809" s="3" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="C809" s="3" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="D809" s="1" t="s">
         <v>586</v>
@@ -38450,10 +38465,10 @@
         <v>808</v>
       </c>
       <c r="B810" s="3" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="C810" s="3" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="D810" s="1" t="s">
         <v>401</v>
@@ -38470,10 +38485,10 @@
         <v>809</v>
       </c>
       <c r="B811" s="3" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="C811" s="3" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="D811" s="1" t="s">
         <v>37</v>
@@ -38490,10 +38505,10 @@
         <v>810</v>
       </c>
       <c r="B812" s="3" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="C812" s="3" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="D812" s="1" t="s">
         <v>24</v>
@@ -38510,7 +38525,7 @@
         <v>811</v>
       </c>
       <c r="B813" s="3" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="C813" s="1" t="s">
         <v>984</v>
@@ -38530,10 +38545,10 @@
         <v>812</v>
       </c>
       <c r="B814" s="3" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="C814" s="3" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="D814" s="1" t="s">
         <v>24</v>
@@ -38550,10 +38565,10 @@
         <v>813</v>
       </c>
       <c r="B815" s="3" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="C815" s="3" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="D815" s="1" t="s">
         <v>105</v>
@@ -38570,10 +38585,10 @@
         <v>814</v>
       </c>
       <c r="B816" s="3" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="C816" s="3" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="D816" s="1" t="s">
         <v>64</v>
@@ -38590,10 +38605,10 @@
         <v>815</v>
       </c>
       <c r="B817" s="3" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="C817" s="3" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="D817" s="1" t="s">
         <v>27</v>
@@ -38610,10 +38625,10 @@
         <v>816</v>
       </c>
       <c r="B818" s="3" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="C818" s="3" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="D818" s="1" t="s">
         <v>162</v>
@@ -38630,10 +38645,10 @@
         <v>817</v>
       </c>
       <c r="B819" s="3" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="C819" s="3" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="D819" s="1" t="s">
         <v>105</v>
@@ -38650,10 +38665,10 @@
         <v>818</v>
       </c>
       <c r="B820" s="3" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="C820" s="3" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="D820" s="1" t="s">
         <v>563</v>
@@ -38670,10 +38685,10 @@
         <v>819</v>
       </c>
       <c r="B821" s="3" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="C821" s="3" t="s">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="D821" s="1" t="s">
         <v>21</v>
@@ -38690,10 +38705,10 @@
         <v>820</v>
       </c>
       <c r="B822" s="3" t="s">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="C822" s="3" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="D822" s="1" t="s">
         <v>34</v>
@@ -38710,10 +38725,10 @@
         <v>821</v>
       </c>
       <c r="B823" s="3" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="C823" s="3" t="s">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="D823" s="1" t="s">
         <v>98</v>
@@ -38730,10 +38745,10 @@
         <v>822</v>
       </c>
       <c r="B824" s="3" t="s">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="C824" s="3" t="s">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="D824" s="1" t="s">
         <v>674</v>
@@ -38756,10 +38771,10 @@
         <v>823</v>
       </c>
       <c r="B825" s="3" t="s">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="C825" s="3" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="D825" s="1" t="s">
         <v>115</v>
@@ -38776,10 +38791,10 @@
         <v>824</v>
       </c>
       <c r="B826" s="3" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="C826" s="3" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="D826" s="1" t="s">
         <v>563</v>
@@ -38796,10 +38811,10 @@
         <v>825</v>
       </c>
       <c r="B827" s="3" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="C827" s="3" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="D827" s="1" t="s">
         <v>24</v>
@@ -38816,10 +38831,10 @@
         <v>826</v>
       </c>
       <c r="B828" s="3" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="C828" s="3" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="D828" s="1" t="s">
         <v>61</v>
@@ -38836,10 +38851,10 @@
         <v>827</v>
       </c>
       <c r="B829" s="3" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="C829" s="3" t="s">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="D829" s="1" t="s">
         <v>52</v>
@@ -38856,7 +38871,7 @@
         <v>828</v>
       </c>
       <c r="B830" s="3" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="C830" s="1" t="s">
         <v>447</v>
@@ -38876,10 +38891,10 @@
         <v>829</v>
       </c>
       <c r="B831" s="3" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="C831" s="3" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="D831" s="1" t="s">
         <v>24</v>
@@ -38896,10 +38911,10 @@
         <v>830</v>
       </c>
       <c r="B832" s="3" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="C832" s="3" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="D832" s="1" t="s">
         <v>40</v>
@@ -38916,13 +38931,13 @@
         <v>831</v>
       </c>
       <c r="B833" s="3" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="C833" s="3" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="D833" s="1" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="E833" s="1" t="n">
         <v>1</v>
@@ -38940,7 +38955,7 @@
         <v>1</v>
       </c>
       <c r="T833" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="834" customFormat="false" ht="258.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38948,10 +38963,10 @@
         <v>832</v>
       </c>
       <c r="B834" s="3" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="C834" s="3" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="D834" s="1" t="s">
         <v>312</v>
@@ -38968,10 +38983,10 @@
         <v>833</v>
       </c>
       <c r="B835" s="3" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="C835" s="3" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="D835" s="1" t="s">
         <v>141</v>
@@ -38988,10 +39003,10 @@
         <v>834</v>
       </c>
       <c r="B836" s="3" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="C836" s="3" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="D836" s="1" t="s">
         <v>134</v>
@@ -39008,13 +39023,13 @@
         <v>835</v>
       </c>
       <c r="B837" s="3" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="C837" s="3" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="D837" s="1" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="E837" s="1" t="n">
         <v>1</v>
@@ -39025,10 +39040,10 @@
         <v>836</v>
       </c>
       <c r="B838" s="3" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="C838" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="D838" s="1" t="s">
         <v>262</v>
@@ -39045,10 +39060,10 @@
         <v>837</v>
       </c>
       <c r="B839" s="3" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="C839" s="3" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="D839" s="1" t="s">
         <v>262</v>
@@ -39065,10 +39080,10 @@
         <v>838</v>
       </c>
       <c r="B840" s="3" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="C840" s="3" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="D840" s="1" t="s">
         <v>18</v>
@@ -39085,10 +39100,10 @@
         <v>839</v>
       </c>
       <c r="B841" s="3" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="C841" s="3" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="D841" s="1" t="s">
         <v>297</v>
@@ -39102,10 +39117,10 @@
         <v>840</v>
       </c>
       <c r="B842" s="3" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="C842" s="3" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="D842" s="1" t="s">
         <v>489</v>
@@ -39119,10 +39134,10 @@
         <v>841</v>
       </c>
       <c r="B843" s="3" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="C843" s="3" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="D843" s="1" t="s">
         <v>37</v>
@@ -39139,13 +39154,13 @@
         <v>842</v>
       </c>
       <c r="B844" s="3" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="C844" s="3" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="D844" s="1" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="E844" s="1" t="n">
         <v>1</v>
@@ -39156,10 +39171,10 @@
         <v>843</v>
       </c>
       <c r="B845" s="3" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="C845" s="3" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="D845" s="1" t="s">
         <v>110</v>
@@ -39176,13 +39191,13 @@
         <v>844</v>
       </c>
       <c r="B846" s="3" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="C846" s="3" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="D846" s="1" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="E846" s="1" t="n">
         <v>1</v>
@@ -39199,10 +39214,10 @@
         <v>845</v>
       </c>
       <c r="B847" s="3" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="C847" s="3" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="D847" s="1" t="s">
         <v>66</v>
@@ -39216,10 +39231,10 @@
         <v>846</v>
       </c>
       <c r="B848" s="3" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="C848" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="D848" s="1" t="s">
         <v>563</v>
@@ -39236,10 +39251,10 @@
         <v>847</v>
       </c>
       <c r="B849" s="3" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="C849" s="3" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="D849" s="1" t="s">
         <v>37</v>
@@ -39256,13 +39271,13 @@
         <v>848</v>
       </c>
       <c r="B850" s="3" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="C850" s="1" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="D850" s="1" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="E850" s="1" t="n">
         <v>1</v>
@@ -39276,10 +39291,10 @@
         <v>849</v>
       </c>
       <c r="B851" s="3" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="C851" s="3" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="D851" s="1" t="s">
         <v>40</v>
@@ -39296,10 +39311,10 @@
         <v>850</v>
       </c>
       <c r="B852" s="3" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="C852" s="3" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="D852" s="1" t="s">
         <v>69</v>
@@ -39316,10 +39331,10 @@
         <v>851</v>
       </c>
       <c r="B853" s="3" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="C853" s="3" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="D853" s="1" t="s">
         <v>137</v>
@@ -39336,10 +39351,10 @@
         <v>852</v>
       </c>
       <c r="B854" s="3" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="C854" s="3" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="D854" s="1" t="s">
         <v>354</v>
@@ -39353,10 +39368,10 @@
         <v>853</v>
       </c>
       <c r="B855" s="3" t="s">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="C855" s="3" t="s">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="D855" s="1" t="s">
         <v>61</v>
@@ -39373,10 +39388,10 @@
         <v>854</v>
       </c>
       <c r="B856" s="3" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
       <c r="C856" s="3" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="D856" s="1" t="s">
         <v>401</v>
@@ -39393,10 +39408,10 @@
         <v>855</v>
       </c>
       <c r="B857" s="3" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="C857" s="3" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="D857" s="1" t="s">
         <v>489</v>
@@ -39413,10 +39428,10 @@
         <v>856</v>
       </c>
       <c r="B858" s="3" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="C858" s="3" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="D858" s="1" t="s">
         <v>141</v>
@@ -39433,10 +39448,10 @@
         <v>857</v>
       </c>
       <c r="B859" s="3" t="s">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="C859" s="3" t="s">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="D859" s="1" t="s">
         <v>622</v>
@@ -39450,13 +39465,13 @@
         <v>858</v>
       </c>
       <c r="B860" s="3" t="s">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="C860" s="1" t="s">
         <v>372</v>
       </c>
       <c r="D860" s="1" t="s">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="E860" s="1" t="n">
         <v>1</v>
@@ -39470,10 +39485,10 @@
         <v>859</v>
       </c>
       <c r="B861" s="3" t="s">
-        <v>1737</v>
+        <v>1738</v>
       </c>
       <c r="C861" s="3" t="s">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="D861" s="1" t="s">
         <v>1483</v>
@@ -39499,13 +39514,13 @@
         <v>860</v>
       </c>
       <c r="B862" s="3" t="s">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="C862" s="3" t="s">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="D862" s="1" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="E862" s="1" t="n">
         <v>1</v>
@@ -39519,10 +39534,10 @@
         <v>861</v>
       </c>
       <c r="B863" s="3" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="C863" s="3" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="D863" s="1" t="s">
         <v>241</v>
@@ -39536,10 +39551,10 @@
         <v>862</v>
       </c>
       <c r="B864" s="3" t="s">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="C864" s="3" t="s">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="D864" s="1" t="s">
         <v>37</v>
@@ -39556,10 +39571,10 @@
         <v>863</v>
       </c>
       <c r="B865" s="3" t="s">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="C865" s="3" t="s">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="D865" s="1" t="s">
         <v>110</v>
@@ -39576,10 +39591,10 @@
         <v>864</v>
       </c>
       <c r="B866" s="3" t="s">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="C866" s="3" t="s">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="D866" s="1" t="s">
         <v>1256</v>
@@ -39602,10 +39617,10 @@
         <v>865</v>
       </c>
       <c r="B867" s="3" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="C867" s="3" t="s">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="D867" s="1" t="s">
         <v>40</v>
@@ -39622,13 +39637,13 @@
         <v>866</v>
       </c>
       <c r="B868" s="3" t="s">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="C868" s="3" t="s">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="D868" s="1" t="s">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="E868" s="1" t="n">
         <v>1</v>
@@ -39640,6 +39655,9 @@
         <v>1</v>
       </c>
       <c r="L868" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M868" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -39648,10 +39666,10 @@
         <v>867</v>
       </c>
       <c r="B869" s="3" t="s">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="C869" s="3" t="s">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="D869" s="1" t="s">
         <v>141</v>
@@ -39668,10 +39686,10 @@
         <v>868</v>
       </c>
       <c r="B870" s="3" t="s">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="C870" s="3" t="s">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="D870" s="1" t="s">
         <v>84</v>
@@ -39694,13 +39712,13 @@
         <v>869</v>
       </c>
       <c r="B871" s="3" t="s">
-        <v>1758</v>
+        <v>1759</v>
       </c>
       <c r="C871" s="3" t="s">
-        <v>1758</v>
+        <v>1759</v>
       </c>
       <c r="D871" s="1" t="s">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="E871" s="1" t="n">
         <v>1</v>
@@ -39711,10 +39729,10 @@
         <v>870</v>
       </c>
       <c r="B872" s="3" t="s">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="C872" s="3" t="s">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="D872" s="1" t="s">
         <v>115</v>
@@ -39728,13 +39746,13 @@
         <v>871</v>
       </c>
       <c r="B873" s="3" t="s">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="C873" s="3" t="s">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="D873" s="1" t="s">
-        <v>1764</v>
+        <v>1765</v>
       </c>
       <c r="E873" s="1" t="n">
         <v>1</v>
@@ -39757,13 +39775,13 @@
         <v>872</v>
       </c>
       <c r="B874" s="3" t="s">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="C874" s="3" t="s">
-        <v>1766</v>
+        <v>1767</v>
       </c>
       <c r="D874" s="1" t="s">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="E874" s="1" t="n">
         <v>1</v>
@@ -39780,10 +39798,10 @@
         <v>873</v>
       </c>
       <c r="B875" s="3" t="s">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="C875" s="3" t="s">
-        <v>1769</v>
+        <v>1770</v>
       </c>
       <c r="D875" s="1" t="s">
         <v>37</v>
@@ -39800,10 +39818,10 @@
         <v>874</v>
       </c>
       <c r="B876" s="3" t="s">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="C876" s="3" t="s">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="D876" s="1" t="s">
         <v>105</v>
@@ -39820,10 +39838,10 @@
         <v>875</v>
       </c>
       <c r="B877" s="3" t="s">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="C877" s="3" t="s">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="D877" s="1" t="s">
         <v>24</v>
@@ -39840,10 +39858,10 @@
         <v>876</v>
       </c>
       <c r="B878" s="3" t="s">
-        <v>1774</v>
+        <v>1775</v>
       </c>
       <c r="C878" s="3" t="s">
-        <v>1775</v>
+        <v>1776</v>
       </c>
       <c r="D878" s="1" t="s">
         <v>312</v>
@@ -39860,10 +39878,10 @@
         <v>877</v>
       </c>
       <c r="B879" s="3" t="s">
-        <v>1776</v>
+        <v>1777</v>
       </c>
       <c r="C879" s="3" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="D879" s="1" t="s">
         <v>37</v>
@@ -39880,10 +39898,10 @@
         <v>878</v>
       </c>
       <c r="B880" s="3" t="s">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="C880" s="3" t="s">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="D880" s="1" t="s">
         <v>40</v>
@@ -39900,10 +39918,10 @@
         <v>879</v>
       </c>
       <c r="B881" s="3" t="s">
-        <v>1780</v>
+        <v>1781</v>
       </c>
       <c r="C881" s="3" t="s">
-        <v>1781</v>
+        <v>1782</v>
       </c>
       <c r="D881" s="1" t="s">
         <v>21</v>
@@ -39920,10 +39938,10 @@
         <v>880</v>
       </c>
       <c r="B882" s="3" t="s">
-        <v>1782</v>
+        <v>1783</v>
       </c>
       <c r="C882" s="3" t="s">
-        <v>1783</v>
+        <v>1784</v>
       </c>
       <c r="D882" s="1" t="s">
         <v>37</v>
@@ -39970,7 +39988,7 @@
       </c>
       <c r="M883" s="1" t="n">
         <f aca="false">SUM(M1:M882)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N883" s="1" t="n">
         <f aca="false">SUM(N1:N882)</f>
@@ -39978,11 +39996,11 @@
       </c>
       <c r="O883" s="1" t="n">
         <f aca="false">SUM(O1:O882)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P883" s="1" t="n">
         <f aca="false">SUM(P1:P882)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q883" s="1" t="n">
         <f aca="false">SUM(Q1:Q882)</f>
@@ -40017,7 +40035,7 @@
       </c>
       <c r="M884" s="5" t="n">
         <f aca="false">M883/881</f>
-        <v>0.0113507377979569</v>
+        <v>0.0124858115777526</v>
       </c>
       <c r="N884" s="5" t="n">
         <f aca="false">N883/881</f>
@@ -40025,11 +40043,11 @@
       </c>
       <c r="O884" s="5" t="n">
         <f aca="false">O883/881</f>
-        <v>0.0147559591373439</v>
+        <v>0.0170261066969353</v>
       </c>
       <c r="P884" s="5" t="n">
         <f aca="false">P883/881</f>
-        <v>0.00113507377979569</v>
+        <v>0</v>
       </c>
       <c r="Q884" s="5" t="n">
         <f aca="false">Q883/881</f>
@@ -40039,7 +40057,7 @@
     <row r="889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H889" s="1" t="n">
         <f aca="false">SUM(F883:I883)+SUM(K883:O883)+Q883</f>
-        <v>911</v>
+        <v>914</v>
       </c>
     </row>
   </sheetData>

</xml_diff>